<commit_message>
Using new OpAmp, re-did layout
</commit_message>
<xml_diff>
--- a/Hardware/Fabrication/Rev C0/BOM/Bill of Materials-WalkMod C0.xlsx
+++ b/Hardware/Fabrication/Rev C0/BOM/Bill of Materials-WalkMod C0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\electronics\pcb_projects\jobs\WalkMod\Hardware\Fabrication\Rev C0\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F9E461F-AE98-4665-942B-4125B0D1F840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AE18AA1-447F-4A0A-BE6D-7E6C7696C666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39540" yWindow="1140" windowWidth="28800" windowHeight="15560" xr2:uid="{87C152A9-9812-49A8-BF1D-D78D75123F6C}"/>
+    <workbookView xWindow="39540" yWindow="1140" windowWidth="28800" windowHeight="15560" xr2:uid="{C0A1DB35-3A35-4C96-91F9-7CD5BE0CBD2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WalkMod C0" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <t>Note</t>
   </si>
   <si>
-    <t>C1, C4, C5</t>
+    <t>C1, C4</t>
   </si>
   <si>
     <t>CL10B105KA8NFNC</t>
@@ -199,13 +199,13 @@
     <t>U2</t>
   </si>
   <si>
-    <t>TLV9004SIRTER</t>
-  </si>
-  <si>
-    <t>WQFN-16_3X3_0.5_C</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
+    <t>LTC2068HUD#PBF</t>
+  </si>
+  <si>
+    <t>QFN16_0.5_C</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF049D77-76A8-4BD3-9124-451B1D3A9B3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1553AEEC-F041-47A3-89C3-D73115EC8BCC}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -642,7 +642,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>

</xml_diff>